<commit_message>
Adicionando Relatório de MTPA4 em LaTex
</commit_message>
<xml_diff>
--- a/Documentacao/Cronograma.xlsx
+++ b/Documentacao/Cronograma.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjetosAula\DowJonesSkins\Documentacao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrey\Desktop\DowJonesSkins\Documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA2F30AD-3C6F-4B71-BF5A-1F39370B5B1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3255EE1-F99C-4BD1-9713-B5D9AB1ECAB5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6014D658-B1D6-4F58-9932-24AC66A47ED0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6014D658-B1D6-4F58-9932-24AC66A47ED0}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -111,7 +111,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -119,14 +119,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="17" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,143 +457,159 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB96CE93-C877-4051-BC44-1BD91BAF16FC}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="B2:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.42578125" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="2" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="2:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="C3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="C4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="C5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="C6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="C7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="C8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="C9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="F9" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="C10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="F10" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" s="3"/>
+      <c r="D11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E11" s="3"/>
+      <c r="F11" s="3" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>